<commit_message>
New summary visualizations for household and industrial categories
</commit_message>
<xml_diff>
--- a/waste_flow/extra_data_xls/waste_to_full_name.xlsx
+++ b/waste_flow/extra_data_xls/waste_to_full_name.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27880" yWindow="460" windowWidth="23120" windowHeight="13580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51120" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
   <si>
     <t>W072</t>
   </si>
@@ -153,6 +153,33 @@
   </si>
   <si>
     <t>W7376_hh</t>
+  </si>
+  <si>
+    <t>plot_color</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>cyan</t>
+  </si>
+  <si>
+    <t>pink</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>black</t>
   </si>
 </sst>
 </file>
@@ -516,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,7 +557,7 @@
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -543,8 +570,11 @@
       <c r="D1" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -557,8 +587,11 @@
       <c r="D2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -571,8 +604,11 @@
       <c r="D3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -585,8 +621,11 @@
       <c r="D4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -599,8 +638,11 @@
       <c r="D5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -613,8 +655,11 @@
       <c r="D6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -627,8 +672,11 @@
       <c r="D7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -641,8 +689,11 @@
       <c r="D8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -655,8 +706,11 @@
       <c r="D9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -669,8 +723,11 @@
       <c r="D10">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -683,8 +740,11 @@
       <c r="D11">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -697,8 +757,11 @@
       <c r="D12">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -711,8 +774,11 @@
       <c r="D13">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -725,8 +791,11 @@
       <c r="D14">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -739,8 +808,11 @@
       <c r="D15">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -753,8 +825,11 @@
       <c r="D16">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -767,8 +842,11 @@
       <c r="D17">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -781,8 +859,11 @@
       <c r="D18">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -795,8 +876,11 @@
       <c r="D19">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -809,8 +893,11 @@
       <c r="D20">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -823,8 +910,11 @@
       <c r="D21">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -836,6 +926,9 @@
       </c>
       <c r="D22">
         <v>0.06</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>